<commit_message>
Added folder organization for codebase
</commit_message>
<xml_diff>
--- a/project_workflow.xlsx
+++ b/project_workflow.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Frank/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Frank/Commodity_TS_Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{73E0A6F8-C8E1-A24E-A072-0DE8AE0DCDC6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ECFAD9C-FA76-4946-A2AD-FF57B7E0A759}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28960" yWindow="2460" windowWidth="25440" windowHeight="15020" xr2:uid="{3570CEE8-FB1D-1341-8149-D16F389D8044}"/>
   </bookViews>
@@ -22,10 +22,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -113,7 +109,10 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
         </a:solidFill>
         <a:ln w="9525" cmpd="sng">
           <a:solidFill>
@@ -122,6 +121,12 @@
             </a:schemeClr>
           </a:solidFill>
         </a:ln>
+        <a:effectLst>
+          <a:innerShdw blurRad="114300">
+            <a:prstClr val="black"/>
+          </a:innerShdw>
+          <a:softEdge rad="38100"/>
+        </a:effectLst>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="0">
@@ -182,11 +187,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
+      <xdr:colOff>25400</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2209800" cy="1854200"/>
+    <xdr:ext cx="2374900" cy="1981200"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="3" name="TextBox 2">
@@ -200,14 +205,17 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4559300" y="736600"/>
-          <a:ext cx="2209800" cy="1854200"/>
+          <a:off x="4152900" y="635000"/>
+          <a:ext cx="2374900" cy="1981200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
         </a:solidFill>
         <a:ln w="9525" cmpd="sng">
           <a:solidFill>
@@ -216,6 +224,12 @@
             </a:schemeClr>
           </a:solidFill>
         </a:ln>
+        <a:effectLst>
+          <a:innerShdw blurRad="114300">
+            <a:prstClr val="black"/>
+          </a:innerShdw>
+          <a:softEdge rad="38100"/>
+        </a:effectLst>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="0">
@@ -269,16 +283,16 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -293,14 +307,17 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7823200" y="723900"/>
+          <a:off x="7289800" y="673100"/>
           <a:ext cx="2336800" cy="1905000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
         </a:solidFill>
         <a:ln w="9525" cmpd="sng">
           <a:solidFill>
@@ -309,6 +326,12 @@
             </a:schemeClr>
           </a:solidFill>
         </a:ln>
+        <a:effectLst>
+          <a:innerShdw blurRad="114300">
+            <a:prstClr val="black"/>
+          </a:innerShdw>
+          <a:softEdge rad="38100"/>
+        </a:effectLst>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="0">
@@ -371,7 +394,10 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
         </a:solidFill>
         <a:ln w="9525" cmpd="sng">
           <a:solidFill>
@@ -380,6 +406,12 @@
             </a:schemeClr>
           </a:solidFill>
         </a:ln>
+        <a:effectLst>
+          <a:innerShdw blurRad="114300">
+            <a:prstClr val="black"/>
+          </a:innerShdw>
+          <a:softEdge rad="38100"/>
+        </a:effectLst>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="0">
@@ -426,16 +458,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -450,14 +482,17 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6172200" y="3530600"/>
+          <a:off x="5702300" y="2743200"/>
           <a:ext cx="2768600" cy="2171700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
         </a:solidFill>
         <a:ln w="9525" cmpd="sng">
           <a:solidFill>
@@ -466,6 +501,12 @@
             </a:schemeClr>
           </a:solidFill>
         </a:ln>
+        <a:effectLst>
+          <a:innerShdw blurRad="114300">
+            <a:prstClr val="black"/>
+          </a:innerShdw>
+          <a:softEdge rad="38100"/>
+        </a:effectLst>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="0">
@@ -497,16 +538,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -521,14 +562,17 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10477500" y="3429000"/>
+          <a:off x="5435600" y="5181600"/>
           <a:ext cx="2387600" cy="2324100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
         </a:solidFill>
         <a:ln w="9525" cmpd="sng">
           <a:solidFill>
@@ -537,6 +581,12 @@
             </a:schemeClr>
           </a:solidFill>
         </a:ln>
+        <a:effectLst>
+          <a:innerShdw blurRad="114300">
+            <a:prstClr val="black"/>
+          </a:innerShdw>
+          <a:softEdge rad="38100"/>
+        </a:effectLst>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="0">
@@ -561,6 +611,306 @@
             <a:rPr lang="en-US" sz="1100"/>
             <a:t>Time-series Analysis</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Right Arrow 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B107294B-90F3-F94E-9397-0E51583EAE83}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="1460500"/>
+          <a:ext cx="558800" cy="368300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Right Arrow 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA11BE44-E242-E640-938B-55AB8E09BBAA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6680200" y="1460500"/>
+          <a:ext cx="495300" cy="406400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Right Arrow 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D06578FE-4693-E843-A717-22CE0281B594}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="20188180">
+          <a:off x="4330700" y="4152900"/>
+          <a:ext cx="495300" cy="406400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Right Arrow 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5383FF6-5843-9C47-9230-9D09396FE9FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="1875845">
+          <a:off x="4305300" y="5003800"/>
+          <a:ext cx="495300" cy="406400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Right Arrow 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{972A717C-F688-DA4C-B912-245262F8B905}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9906000" y="1625600"/>
+          <a:ext cx="495300" cy="406400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -904,7 +1254,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>